<commit_message>
Changes for Palviainen et al 2024
</commit_message>
<xml_diff>
--- a/inputs/susi_motti_input_lyr_0.xlsx
+++ b/inputs/susi_motti_input_lyr_0.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuef-my.sharepoint.com/personal/alauren_uef_fi/Documents/codes/Susi_10/inputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_46FE7781AAF727E17BE69C661FB721CF03D9A5B7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16D62F25-39D6-40DA-93B0-C272CB0E6CBC}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StandData" sheetId="1" r:id="rId1"/>
     <sheet name="Kertymät" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -95,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +178,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -205,7 +232,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +264,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,6 +316,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,14 +509,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,7 +586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -532,22 +597,22 @@
         <v>35</v>
       </c>
       <c r="D2">
-        <v>999.9906005859359</v>
+        <v>999.99060058593591</v>
       </c>
       <c r="E2">
-        <v>5.997855713663347</v>
+        <v>5.9978557136633466</v>
       </c>
       <c r="F2">
-        <v>9.321612490522059</v>
+        <v>9.3216124905220585</v>
       </c>
       <c r="G2">
-        <v>11.20916609193696</v>
+        <v>11.209166091936959</v>
       </c>
       <c r="H2">
-        <v>9.321612490522059</v>
+        <v>9.3216124905220585</v>
       </c>
       <c r="I2">
-        <v>30.15510787292036</v>
+        <v>30.155107872920361</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -556,25 +621,25 @@
         <v>24.51946729223377</v>
       </c>
       <c r="L2">
-        <v>5.635641104550611</v>
+        <v>5.6356411045506114</v>
       </c>
       <c r="M2">
-        <v>30.15510787292036</v>
+        <v>30.155107872920361</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>9.329977758139233</v>
+        <v>9.3299777581392327</v>
       </c>
       <c r="P2">
-        <v>2.252557300499305</v>
+        <v>2.2525573004993049</v>
       </c>
       <c r="Q2">
-        <v>3.327035213760185</v>
+        <v>3.3270352137601851</v>
       </c>
       <c r="R2">
-        <v>0.8159891120749043</v>
+        <v>0.81598911207490432</v>
       </c>
       <c r="S2">
         <v>1.683233137571255</v>
@@ -583,13 +648,13 @@
         <v>1.021726469932881</v>
       </c>
       <c r="U2">
-        <v>2.517646219051367</v>
+        <v>2.5176462190513669</v>
       </c>
       <c r="V2">
-        <v>0.06665603262407602</v>
+        <v>6.6656032624076017E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -600,52 +665,52 @@
         <v>40</v>
       </c>
       <c r="D3">
-        <v>980.6843261718751</v>
+        <v>980.68432617187511</v>
       </c>
       <c r="E3">
-        <v>8.36077177633897</v>
+        <v>8.3607717763389697</v>
       </c>
       <c r="F3">
         <v>10.99052767875415</v>
       </c>
       <c r="G3">
-        <v>12.83582353886642</v>
+        <v>12.835823538866419</v>
       </c>
       <c r="H3">
         <v>10.99052767875415</v>
       </c>
       <c r="I3">
-        <v>48.25287318057312</v>
+        <v>48.252873180573118</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>42.38587363933808</v>
+        <v>42.385873639338079</v>
       </c>
       <c r="L3">
-        <v>5.86699945682477</v>
+        <v>5.8669994568247699</v>
       </c>
       <c r="M3">
-        <v>48.25287318057312</v>
+        <v>48.252873180573118</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>16.32091138748081</v>
+        <v>16.320911387480809</v>
       </c>
       <c r="P3">
-        <v>2.358237098194319</v>
+        <v>2.3582370981943188</v>
       </c>
       <c r="Q3">
-        <v>4.756840917472744</v>
+        <v>4.7568409174727444</v>
       </c>
       <c r="R3">
         <v>1.182784583551592</v>
       </c>
       <c r="S3">
-        <v>2.286894544222959</v>
+        <v>2.2868945442229589</v>
       </c>
       <c r="T3">
         <v>1.554073164269836</v>
@@ -657,7 +722,7 @@
         <v>0.1111430704052664</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -674,58 +739,58 @@
         <v>10.92012513330118</v>
       </c>
       <c r="F4">
-        <v>12.62139104110324</v>
+        <v>12.621391041103241</v>
       </c>
       <c r="G4">
         <v>14.39495854225857</v>
       </c>
       <c r="H4">
-        <v>12.62139104110324</v>
+        <v>12.621391041103241</v>
       </c>
       <c r="I4">
-        <v>70.99213438479028</v>
+        <v>70.992134384790276</v>
       </c>
       <c r="J4">
-        <v>4.984664768197623</v>
+        <v>4.9846647681976233</v>
       </c>
       <c r="K4">
         <v>60.86327177299561</v>
       </c>
       <c r="L4">
-        <v>5.144198404253424</v>
+        <v>5.1441984042534239</v>
       </c>
       <c r="M4">
-        <v>70.99213438479028</v>
+        <v>70.992134384790276</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>25.56844493617358</v>
+        <v>25.568444936173581</v>
       </c>
       <c r="P4">
-        <v>2.073336858493586</v>
+        <v>2.0733368584935858</v>
       </c>
       <c r="Q4">
         <v>6.249623789505403</v>
       </c>
       <c r="R4">
-        <v>1.604778566967659</v>
+        <v>1.6047785669676591</v>
       </c>
       <c r="S4">
-        <v>2.879561348895839</v>
+        <v>2.8795613488958391</v>
       </c>
       <c r="T4">
-        <v>2.184027513301411</v>
+        <v>2.1840275133014111</v>
       </c>
       <c r="U4">
-        <v>5.73645973431734</v>
+        <v>5.7364597343173402</v>
       </c>
       <c r="V4">
         <v>0.1658627296929967</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -736,64 +801,64 @@
         <v>50</v>
       </c>
       <c r="D5">
-        <v>945.294830322266</v>
+        <v>945.29483032226597</v>
       </c>
       <c r="E5">
         <v>13.333159725798</v>
       </c>
       <c r="F5">
-        <v>14.18839534438533</v>
+        <v>14.188395344385331</v>
       </c>
       <c r="G5">
         <v>15.76999222966049</v>
       </c>
       <c r="H5">
-        <v>14.18839534438533</v>
+        <v>14.188395344385331</v>
       </c>
       <c r="I5">
-        <v>95.93696497540304</v>
+        <v>95.936964975403043</v>
       </c>
       <c r="J5">
         <v>10.1068490774437</v>
       </c>
       <c r="K5">
-        <v>81.74250760213798</v>
+        <v>81.742507602137977</v>
       </c>
       <c r="L5">
-        <v>4.087609215377284</v>
+        <v>4.0876092153772836</v>
       </c>
       <c r="M5">
-        <v>95.93696497540304</v>
+        <v>95.936964975403043</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>35.90552420853695</v>
+        <v>35.905524208536953</v>
       </c>
       <c r="P5">
-        <v>1.646269884621392</v>
+        <v>1.6462698846213919</v>
       </c>
       <c r="Q5">
-        <v>7.548380782989049</v>
+        <v>7.5483807829890486</v>
       </c>
       <c r="R5">
-        <v>2.022704281637908</v>
+        <v>2.0227042816379082</v>
       </c>
       <c r="S5">
-        <v>3.369072153239258</v>
+        <v>3.3690721532392578</v>
       </c>
       <c r="T5">
         <v>2.821126764111018</v>
       </c>
       <c r="U5">
-        <v>7.611172058801687</v>
+        <v>7.6111720588016869</v>
       </c>
       <c r="V5">
         <v>0.224380206849806</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -804,16 +869,16 @@
         <v>55</v>
       </c>
       <c r="D6">
-        <v>924.5821838378902</v>
+        <v>924.58218383789017</v>
       </c>
       <c r="E6">
-        <v>15.74179495481101</v>
+        <v>15.741794954811009</v>
       </c>
       <c r="F6">
         <v>15.66588198831611</v>
       </c>
       <c r="G6">
-        <v>17.09573584658695</v>
+        <v>17.095735846586951</v>
       </c>
       <c r="H6">
         <v>15.66588198831611</v>
@@ -825,10 +890,10 @@
         <v>29.50771985404938</v>
       </c>
       <c r="K6">
-        <v>89.62879854761941</v>
+        <v>89.628798547619411</v>
       </c>
       <c r="L6">
-        <v>4.113122490366925</v>
+        <v>4.1131224903669246</v>
       </c>
       <c r="M6">
         <v>123.2496415585539</v>
@@ -840,16 +905,16 @@
         <v>46.78434668398603</v>
       </c>
       <c r="P6">
-        <v>1.661978136663273</v>
+        <v>1.6619781366632731</v>
       </c>
       <c r="Q6">
-        <v>8.716415026107532</v>
+        <v>8.7164150261075317</v>
       </c>
       <c r="R6">
-        <v>2.456477943320284</v>
+        <v>2.4564779433202841</v>
       </c>
       <c r="S6">
-        <v>3.770932637654227</v>
+        <v>3.7709326376542269</v>
       </c>
       <c r="T6">
         <v>3.492524760415344</v>
@@ -858,10 +923,10 @@
         <v>9.662915038519392</v>
       </c>
       <c r="V6">
-        <v>0.2850825079941519</v>
+        <v>0.28508250799415191</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -872,31 +937,31 @@
         <v>60</v>
       </c>
       <c r="D7">
-        <v>900.2477111816411</v>
+        <v>900.24771118164108</v>
       </c>
       <c r="E7">
         <v>18.16163974339943</v>
       </c>
       <c r="F7">
-        <v>17.04589695024095</v>
+        <v>17.045896950240952</v>
       </c>
       <c r="G7">
         <v>18.41865302696721</v>
       </c>
       <c r="H7">
-        <v>17.04589695024095</v>
+        <v>17.045896950240952</v>
       </c>
       <c r="I7">
         <v>152.4332115696775</v>
       </c>
       <c r="J7">
-        <v>44.07787571998144</v>
+        <v>44.077875719981442</v>
       </c>
       <c r="K7">
         <v>104.1777659571855</v>
       </c>
       <c r="L7">
-        <v>4.177569976291131</v>
+        <v>4.1775699762911307</v>
       </c>
       <c r="M7">
         <v>152.4332115696775</v>
@@ -905,31 +970,31 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>58.42184492176351</v>
+        <v>58.421844921763508</v>
       </c>
       <c r="P7">
-        <v>1.693122917945662</v>
+        <v>1.6931229179456619</v>
       </c>
       <c r="Q7">
         <v>9.747581697651027</v>
       </c>
       <c r="R7">
-        <v>2.907118869579914</v>
+        <v>2.9071188695799139</v>
       </c>
       <c r="S7">
-        <v>4.076846660321426</v>
+        <v>4.0768466603214257</v>
       </c>
       <c r="T7">
-        <v>4.198614803464243</v>
+        <v>4.1986148034642428</v>
       </c>
       <c r="U7">
-        <v>11.90341903336594</v>
+        <v>11.903419033365941</v>
       </c>
       <c r="V7">
-        <v>0.3449012218003982</v>
+        <v>0.34490122180039823</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -940,64 +1005,64 @@
         <v>65</v>
       </c>
       <c r="D8">
-        <v>870.6379547119138</v>
+        <v>870.63795471191384</v>
       </c>
       <c r="E8">
         <v>20.36648761415946</v>
       </c>
       <c r="F8">
-        <v>18.3268554820092</v>
+        <v>18.326855482009201</v>
       </c>
       <c r="G8">
-        <v>19.68579754445445</v>
+        <v>19.685797544454449</v>
       </c>
       <c r="H8">
-        <v>18.3268554820092</v>
+        <v>18.326855482009201</v>
       </c>
       <c r="I8">
-        <v>181.0632931717595</v>
+        <v>181.06329317175951</v>
       </c>
       <c r="J8">
-        <v>66.5525887197382</v>
+        <v>66.552588719738196</v>
       </c>
       <c r="K8">
         <v>110.2685817486244</v>
       </c>
       <c r="L8">
-        <v>4.242126646205278</v>
+        <v>4.2421266462052776</v>
       </c>
       <c r="M8">
-        <v>181.0632931717595</v>
+        <v>181.06329317175951</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
       <c r="O8">
-        <v>69.88495690476205</v>
+        <v>69.884956904762049</v>
       </c>
       <c r="P8">
         <v>1.7241567725117</v>
       </c>
       <c r="Q8">
-        <v>10.57482822100268</v>
+        <v>10.574828221002679</v>
       </c>
       <c r="R8">
-        <v>3.331657491278322</v>
+        <v>3.3316574912783219</v>
       </c>
       <c r="S8">
-        <v>4.281561591927035</v>
+        <v>4.2815615919270353</v>
       </c>
       <c r="T8">
-        <v>4.871821993544475</v>
+        <v>4.8718219935444749</v>
       </c>
       <c r="U8">
-        <v>14.12830640069073</v>
+        <v>14.128306400690731</v>
       </c>
       <c r="V8">
-        <v>0.4007541677325145</v>
+        <v>0.40075416773251449</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1011,37 +1076,37 @@
         <v>836.0265502929692</v>
       </c>
       <c r="E9">
-        <v>22.3266183199348</v>
+        <v>22.326618319934799</v>
       </c>
       <c r="F9">
-        <v>19.51543390335535</v>
+        <v>19.515433903355351</v>
       </c>
       <c r="G9">
-        <v>20.91010925358431</v>
+        <v>20.910109253584309</v>
       </c>
       <c r="H9">
-        <v>19.51543390335535</v>
+        <v>19.515433903355351</v>
       </c>
       <c r="I9">
-        <v>208.2726153839581</v>
+        <v>208.27261538395811</v>
       </c>
       <c r="J9">
-        <v>88.79451648176993</v>
+        <v>88.794516481769932</v>
       </c>
       <c r="K9">
         <v>116.1590814351657</v>
       </c>
       <c r="L9">
-        <v>3.319014611985521</v>
+        <v>3.3190146119855211</v>
       </c>
       <c r="M9">
-        <v>208.2726153839581</v>
+        <v>208.27261538395811</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <v>81.2300842438146</v>
+        <v>81.230084243814602</v>
       </c>
       <c r="P9">
         <v>1.343985983007707</v>
@@ -1050,22 +1115,22 @@
         <v>11.22144287250425</v>
       </c>
       <c r="R9">
-        <v>3.720900754263026</v>
+        <v>3.7209007542630261</v>
       </c>
       <c r="S9">
         <v>4.401456307938977</v>
       </c>
       <c r="T9">
-        <v>5.495736590460429</v>
+        <v>5.4957365904604289</v>
       </c>
       <c r="U9">
-        <v>16.2780162869387</v>
+        <v>16.278016286938701</v>
       </c>
       <c r="V9">
         <v>0.4515894040547424</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1076,34 +1141,34 @@
         <v>75</v>
       </c>
       <c r="D10">
-        <v>792.9659271240229</v>
+        <v>792.96592712402287</v>
       </c>
       <c r="E10">
         <v>23.88842293786956</v>
       </c>
       <c r="F10">
-        <v>20.61810975826645</v>
+        <v>20.618109758266449</v>
       </c>
       <c r="G10">
-        <v>22.10319809126935</v>
+        <v>22.103198091269348</v>
       </c>
       <c r="H10">
-        <v>20.61810975826645</v>
+        <v>20.618109758266449</v>
       </c>
       <c r="I10">
-        <v>231.9905500826391</v>
+        <v>231.99055008263909</v>
       </c>
       <c r="J10">
         <v>120.3141937770196</v>
       </c>
       <c r="K10">
-        <v>108.666871521805</v>
+        <v>108.66687152180501</v>
       </c>
       <c r="L10">
-        <v>3.009487121348518</v>
+        <v>3.0094871213485179</v>
       </c>
       <c r="M10">
-        <v>231.9905500826391</v>
+        <v>231.99055008263909</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1112,16 +1177,16 @@
         <v>90.95772194866673</v>
       </c>
       <c r="P10">
-        <v>1.21902154175195</v>
+        <v>1.2190215417519501</v>
       </c>
       <c r="Q10">
-        <v>11.667680605276</v>
+        <v>11.667680605276001</v>
       </c>
       <c r="R10">
         <v>4.045254761605884</v>
       </c>
       <c r="S10">
-        <v>4.436183314096492</v>
+        <v>4.4361833140964917</v>
       </c>
       <c r="T10">
         <v>6.02395930253779</v>
@@ -1130,10 +1195,10 @@
         <v>18.20101952801269</v>
       </c>
       <c r="V10">
-        <v>0.4950780577268613</v>
+        <v>0.49507805772686131</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1144,16 +1209,16 @@
         <v>80</v>
       </c>
       <c r="D11">
-        <v>721.0408592224123</v>
+        <v>721.04085922241234</v>
       </c>
       <c r="E11">
-        <v>24.252526829886</v>
+        <v>24.252526829886001</v>
       </c>
       <c r="F11">
         <v>21.63576567390534</v>
       </c>
       <c r="G11">
-        <v>23.26927475469965</v>
+        <v>23.269274754699651</v>
       </c>
       <c r="H11">
         <v>21.63576567390534</v>
@@ -1162,10 +1227,10 @@
         <v>243.6156057446218</v>
       </c>
       <c r="J11">
-        <v>134.9519210734383</v>
+        <v>134.95192107343831</v>
       </c>
       <c r="K11">
-        <v>106.0336698801322</v>
+        <v>106.03366988013219</v>
       </c>
       <c r="L11">
         <v>2.630012986280255</v>
@@ -1177,31 +1242,31 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>95.91399325373386</v>
+        <v>95.913993253733864</v>
       </c>
       <c r="P11">
         <v>1.065712073592302</v>
       </c>
       <c r="Q11">
-        <v>11.80829075882349</v>
+        <v>11.808290758823491</v>
       </c>
       <c r="R11">
-        <v>4.163049543176852</v>
+        <v>4.1630495431768519</v>
       </c>
       <c r="S11">
-        <v>4.365202664376877</v>
+        <v>4.3652026643768771</v>
       </c>
       <c r="T11">
-        <v>6.241179342882131</v>
+        <v>6.2411793428821314</v>
       </c>
       <c r="U11">
         <v>19.21510069689575</v>
       </c>
       <c r="V11">
-        <v>0.5264434289281412</v>
+        <v>0.52644342892814122</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1212,34 +1277,34 @@
         <v>85</v>
       </c>
       <c r="D12">
-        <v>658.7685890197752</v>
+        <v>658.76858901977516</v>
       </c>
       <c r="E12">
-        <v>24.55855054963184</v>
+        <v>24.558550549631839</v>
       </c>
       <c r="F12">
-        <v>22.58741759675211</v>
+        <v>22.587417596752111</v>
       </c>
       <c r="G12">
         <v>24.41991147027769</v>
       </c>
       <c r="H12">
-        <v>22.58741759675211</v>
+        <v>22.587417596752111</v>
       </c>
       <c r="I12">
-        <v>253.9566125054976</v>
+        <v>253.95661250549759</v>
       </c>
       <c r="J12">
         <v>155.3429004649708</v>
       </c>
       <c r="K12">
-        <v>96.29213265347805</v>
+        <v>96.292132653478049</v>
       </c>
       <c r="L12">
         <v>2.321582309109703</v>
       </c>
       <c r="M12">
-        <v>253.9566125054976</v>
+        <v>253.95661250549759</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1248,25 +1313,25 @@
         <v>100.3246846010491</v>
       </c>
       <c r="P12">
-        <v>0.9411232977350859</v>
+        <v>0.94112329773508585</v>
       </c>
       <c r="Q12">
-        <v>11.90415583348251</v>
+        <v>11.904155833482511</v>
       </c>
       <c r="R12">
         <v>4.264812766439058</v>
       </c>
       <c r="S12">
-        <v>4.280354544904284</v>
+        <v>4.2803545449042844</v>
       </c>
       <c r="T12">
-        <v>6.429683512581904</v>
+        <v>6.4296835125819038</v>
       </c>
       <c r="U12">
         <v>20.1529732948581</v>
       </c>
       <c r="V12">
-        <v>0.5547339400209271</v>
+        <v>0.55473394002092713</v>
       </c>
     </row>
   </sheetData>
@@ -1275,14 +1340,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>

</xml_diff>